<commit_message>
bug fixes in get_pf_shortcircuit_results.py (results at fault location are now extracted correctly); added new excel files with correct bus results
</commit_message>
<xml_diff>
--- a/pandapower/test/shortcircuit/SCE_Tests/sc_result_comparison/test_case_2_five_bus_radial_grid_dyn_gen_pf_sc_results_1_branch.xlsx
+++ b/pandapower/test/shortcircuit/SCE_Tests/sc_result_comparison/test_case_2_five_bus_radial_grid_dyn_gen_pf_sc_results_1_branch.xlsx
@@ -652,52 +652,52 @@
         <v>17</v>
       </c>
       <c r="B2">
-        <v>0.1732050000389407</v>
+        <v>0.1732050000389575</v>
       </c>
       <c r="C2">
-        <v>0.1732050000389407</v>
+        <v>0.1732050000389575</v>
       </c>
       <c r="D2">
-        <v>0.2449488601259024</v>
+        <v>0.2449488601259261</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>5.999997203848292</v>
+        <v>5.999997203848873</v>
       </c>
       <c r="G2">
-        <v>5.999997203848292</v>
+        <v>5.999997203848873</v>
       </c>
       <c r="H2">
         <v>-1E-07</v>
       </c>
       <c r="I2">
-        <v>0.04679995725940969</v>
+        <v>0.04679995725941991</v>
       </c>
       <c r="J2">
         <v>-1E-07</v>
       </c>
       <c r="K2">
-        <v>0.05309995072980261</v>
+        <v>0.05309995072983359</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>-87.32801701726541</v>
+        <v>-87.32801701726295</v>
       </c>
       <c r="N2">
         <v>0</v>
       </c>
       <c r="O2">
-        <v>0.0117967102716749</v>
+        <v>0.01179671027167875</v>
       </c>
       <c r="P2">
         <v>0</v>
       </c>
       <c r="Q2">
-        <v>-38.71954858007843</v>
+        <v>-38.7195485800656</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -705,10 +705,10 @@
         <v>18</v>
       </c>
       <c r="B3">
-        <v>0.1732050000113296</v>
+        <v>0.1732050000113314</v>
       </c>
       <c r="C3">
-        <v>0.1732050000113296</v>
+        <v>0.1732050000113314</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -717,40 +717,40 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>5.999997202891816</v>
+        <v>5.999997202891877</v>
       </c>
       <c r="G3">
-        <v>5.999997202891816</v>
+        <v>5.999997202891877</v>
       </c>
       <c r="H3">
-        <v>0.09359991437045481</v>
+        <v>0.0935999143704609</v>
       </c>
       <c r="I3">
-        <v>-0.04679995703973806</v>
+        <v>-0.04679995703974241</v>
       </c>
       <c r="J3">
-        <v>0.1061999017214356</v>
+        <v>0.1061999017214649</v>
       </c>
       <c r="K3">
-        <v>-0.05309995090837134</v>
+        <v>-0.05309995090839929</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <v>92.67198275374777</v>
+        <v>92.67198275374828</v>
       </c>
       <c r="N3">
-        <v>0.02359342056349899</v>
+        <v>0.02359342056350311</v>
       </c>
       <c r="O3">
-        <v>0.0117967102716749</v>
+        <v>0.01179671027167875</v>
       </c>
       <c r="P3">
-        <v>-38.71954869393782</v>
+        <v>-38.7195486939313</v>
       </c>
       <c r="Q3">
-        <v>-38.71954858007843</v>
+        <v>-38.7195485800656</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -794,16 +794,16 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.0117967102726152</v>
+        <v>0.01179671027261923</v>
       </c>
       <c r="O4">
-        <v>0.0117967102716749</v>
+        <v>0.01179671027167875</v>
       </c>
       <c r="P4">
-        <v>-38.71954846558802</v>
+        <v>-38.7195484655745</v>
       </c>
       <c r="Q4">
-        <v>-38.71954858007843</v>
+        <v>-38.7195485800656</v>
       </c>
     </row>
   </sheetData>
@@ -6247,52 +6247,52 @@
         <v>17</v>
       </c>
       <c r="B2">
-        <v>0.1732050000389407</v>
+        <v>0.1732050000389575</v>
       </c>
       <c r="C2">
-        <v>0.1732050000389407</v>
+        <v>0.1732050000389575</v>
       </c>
       <c r="D2">
-        <v>0.2449488601259024</v>
+        <v>0.2449488601259261</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>5.999997203848292</v>
+        <v>5.999997203848873</v>
       </c>
       <c r="G2">
-        <v>5.999997203848292</v>
+        <v>5.999997203848873</v>
       </c>
       <c r="H2">
         <v>-1E-07</v>
       </c>
       <c r="I2">
-        <v>0.04679995725940969</v>
+        <v>0.04679995725941991</v>
       </c>
       <c r="J2">
         <v>-1E-07</v>
       </c>
       <c r="K2">
-        <v>0.05309995072980261</v>
+        <v>0.05309995072983359</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>-87.32801701726541</v>
+        <v>-87.32801701726295</v>
       </c>
       <c r="N2">
         <v>0</v>
       </c>
       <c r="O2">
-        <v>0.0117967102716749</v>
+        <v>0.01179671027167875</v>
       </c>
       <c r="P2">
         <v>0</v>
       </c>
       <c r="Q2">
-        <v>-38.71954858007843</v>
+        <v>-38.7195485800656</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -6300,10 +6300,10 @@
         <v>18</v>
       </c>
       <c r="B3">
-        <v>0.1732050000113296</v>
+        <v>0.1732050000113314</v>
       </c>
       <c r="C3">
-        <v>0.1732050000113296</v>
+        <v>0.1732050000113314</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -6312,40 +6312,40 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>5.999997202891816</v>
+        <v>5.999997202891877</v>
       </c>
       <c r="G3">
-        <v>5.999997202891816</v>
+        <v>5.999997202891877</v>
       </c>
       <c r="H3">
-        <v>0.09359991437045481</v>
+        <v>0.0935999143704609</v>
       </c>
       <c r="I3">
-        <v>-0.04679995703973806</v>
+        <v>-0.04679995703974241</v>
       </c>
       <c r="J3">
-        <v>0.1061999017214356</v>
+        <v>0.1061999017214649</v>
       </c>
       <c r="K3">
-        <v>-0.05309995090837134</v>
+        <v>-0.05309995090839929</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <v>92.67198275374777</v>
+        <v>92.67198275374828</v>
       </c>
       <c r="N3">
-        <v>0.02359342056349899</v>
+        <v>0.02359342056350311</v>
       </c>
       <c r="O3">
-        <v>0.0117967102716749</v>
+        <v>0.01179671027167875</v>
       </c>
       <c r="P3">
-        <v>-38.71954869393782</v>
+        <v>-38.7195486939313</v>
       </c>
       <c r="Q3">
-        <v>-38.71954858007843</v>
+        <v>-38.7195485800656</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -6389,16 +6389,16 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.0117967102726152</v>
+        <v>0.01179671027261923</v>
       </c>
       <c r="O4">
-        <v>0.0117967102716749</v>
+        <v>0.01179671027167875</v>
       </c>
       <c r="P4">
-        <v>-38.71954846558802</v>
+        <v>-38.7195484655745</v>
       </c>
       <c r="Q4">
-        <v>-38.71954858007843</v>
+        <v>-38.7195485800656</v>
       </c>
     </row>
   </sheetData>
@@ -11842,52 +11842,52 @@
         <v>17</v>
       </c>
       <c r="B2">
-        <v>0.1732049998501529</v>
+        <v>0.1732049998501554</v>
       </c>
       <c r="C2">
-        <v>0.1732049998501529</v>
+        <v>0.1732049998501554</v>
       </c>
       <c r="D2">
-        <v>0.244948859858916</v>
+        <v>0.2449488598589196</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>5.99999719730849</v>
+        <v>5.999997197308577</v>
       </c>
       <c r="G2">
-        <v>5.99999719730849</v>
+        <v>5.999997197308577</v>
       </c>
       <c r="H2">
-        <v>-1.189065189167579</v>
+        <v>-1.189065189167616</v>
       </c>
       <c r="I2">
-        <v>1.235865146411197</v>
+        <v>1.235865146411234</v>
       </c>
       <c r="J2">
-        <v>-5.266440511374123</v>
+        <v>-5.266440511374197</v>
       </c>
       <c r="K2">
-        <v>5.319540462088362</v>
+        <v>5.319540462088439</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>-87.32801729386279</v>
+        <v>-87.32801729386256</v>
       </c>
       <c r="N2">
-        <v>0.8998348446627195</v>
+        <v>0.8998348446627199</v>
       </c>
       <c r="O2">
-        <v>0.9102029879103775</v>
+        <v>0.9102029879103781</v>
       </c>
       <c r="P2">
-        <v>-10.05101633967408</v>
+        <v>-10.05101633967405</v>
       </c>
       <c r="Q2">
-        <v>-10.40726689094585</v>
+        <v>-10.40726689094582</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -11895,10 +11895,10 @@
         <v>18</v>
       </c>
       <c r="B3">
-        <v>0.1732049999484002</v>
+        <v>0.1732049999484007</v>
       </c>
       <c r="C3">
-        <v>0.1732049999484002</v>
+        <v>0.1732049999484007</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -11907,40 +11907,40 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>5.99999720071188</v>
+        <v>5.999997200711895</v>
       </c>
       <c r="G3">
-        <v>5.99999720071188</v>
+        <v>5.999997200711895</v>
       </c>
       <c r="H3">
-        <v>1.282665100269789</v>
+        <v>1.282665100269815</v>
       </c>
       <c r="I3">
-        <v>-1.235865142973079</v>
+        <v>-1.235865142973104</v>
       </c>
       <c r="J3">
-        <v>5.372640416841883</v>
+        <v>5.372640416841895</v>
       </c>
       <c r="K3">
-        <v>-5.319540466067403</v>
+        <v>-5.319540466067416</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <v>92.67198266154801</v>
+        <v>92.67198266154827</v>
       </c>
       <c r="N3">
-        <v>0.920605526532746</v>
+        <v>0.9206055265327466</v>
       </c>
       <c r="O3">
-        <v>0.9102029879103775</v>
+        <v>0.9102029879103781</v>
       </c>
       <c r="P3">
-        <v>-10.75547962562467</v>
+        <v>-10.75547962562463</v>
       </c>
       <c r="Q3">
-        <v>-10.40726689094585</v>
+        <v>-10.40726689094582</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -11984,16 +11984,16 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.9102029879096086</v>
+        <v>0.9102029879096094</v>
       </c>
       <c r="O4">
-        <v>0.9102029879103775</v>
+        <v>0.9102029879103781</v>
       </c>
       <c r="P4">
-        <v>-10.40726689059163</v>
+        <v>-10.40726689059159</v>
       </c>
       <c r="Q4">
-        <v>-10.40726689094585</v>
+        <v>-10.40726689094582</v>
       </c>
     </row>
   </sheetData>
@@ -13678,52 +13678,52 @@
         <v>17</v>
       </c>
       <c r="B2">
-        <v>0.1732049998501529</v>
+        <v>0.1732049998501554</v>
       </c>
       <c r="C2">
-        <v>0.1732049998501529</v>
+        <v>0.1732049998501554</v>
       </c>
       <c r="D2">
-        <v>0.244948859858916</v>
+        <v>0.2449488598589196</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>5.99999719730849</v>
+        <v>5.999997197308577</v>
       </c>
       <c r="G2">
-        <v>5.99999719730849</v>
+        <v>5.999997197308577</v>
       </c>
       <c r="H2">
-        <v>-1.189065189167579</v>
+        <v>-1.189065189167616</v>
       </c>
       <c r="I2">
-        <v>1.235865146411197</v>
+        <v>1.235865146411234</v>
       </c>
       <c r="J2">
-        <v>-5.266440511374123</v>
+        <v>-5.266440511374197</v>
       </c>
       <c r="K2">
-        <v>5.319540462088362</v>
+        <v>5.319540462088439</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>-87.32801729386279</v>
+        <v>-87.32801729386256</v>
       </c>
       <c r="N2">
-        <v>0.8998348446627195</v>
+        <v>0.8998348446627199</v>
       </c>
       <c r="O2">
-        <v>0.9102029879103775</v>
+        <v>0.9102029879103781</v>
       </c>
       <c r="P2">
-        <v>-10.05101633967408</v>
+        <v>-10.05101633967405</v>
       </c>
       <c r="Q2">
-        <v>-10.40726689094585</v>
+        <v>-10.40726689094582</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -13731,10 +13731,10 @@
         <v>18</v>
       </c>
       <c r="B3">
-        <v>0.1732049999484002</v>
+        <v>0.1732049999484007</v>
       </c>
       <c r="C3">
-        <v>0.1732049999484002</v>
+        <v>0.1732049999484007</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -13743,40 +13743,40 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>5.99999720071188</v>
+        <v>5.999997200711895</v>
       </c>
       <c r="G3">
-        <v>5.99999720071188</v>
+        <v>5.999997200711895</v>
       </c>
       <c r="H3">
-        <v>1.282665100269789</v>
+        <v>1.282665100269815</v>
       </c>
       <c r="I3">
-        <v>-1.235865142973079</v>
+        <v>-1.235865142973104</v>
       </c>
       <c r="J3">
-        <v>5.372640416841883</v>
+        <v>5.372640416841895</v>
       </c>
       <c r="K3">
-        <v>-5.319540466067403</v>
+        <v>-5.319540466067416</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <v>92.67198266154801</v>
+        <v>92.67198266154827</v>
       </c>
       <c r="N3">
-        <v>0.920605526532746</v>
+        <v>0.9206055265327466</v>
       </c>
       <c r="O3">
-        <v>0.9102029879103775</v>
+        <v>0.9102029879103781</v>
       </c>
       <c r="P3">
-        <v>-10.75547962562467</v>
+        <v>-10.75547962562463</v>
       </c>
       <c r="Q3">
-        <v>-10.40726689094585</v>
+        <v>-10.40726689094582</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -13820,16 +13820,16 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.9102029879096086</v>
+        <v>0.9102029879096094</v>
       </c>
       <c r="O4">
-        <v>0.9102029879103775</v>
+        <v>0.9102029879103781</v>
       </c>
       <c r="P4">
-        <v>-10.40726689059163</v>
+        <v>-10.40726689059159</v>
       </c>
       <c r="Q4">
-        <v>-10.40726689094585</v>
+        <v>-10.40726689094582</v>
       </c>
     </row>
   </sheetData>
@@ -13909,7 +13909,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1.347221355506749E-09</v>
+        <v>1.347219034915371E-09</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -13921,13 +13921,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>7.279831186286096E-20</v>
+        <v>7.278924918958987E-20</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>2.670423360815112E-19</v>
+        <v>2.670206890999608E-19</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -14134,7 +14134,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1.347221355506749E-09</v>
+        <v>1.347219034915371E-09</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -14146,13 +14146,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>7.279831186286096E-20</v>
+        <v>7.278924918958987E-20</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>2.670423360815112E-19</v>
+        <v>2.670206890999608E-19</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -14359,7 +14359,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>3.617452049950389E-10</v>
+        <v>3.617436737412018E-10</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -14371,13 +14371,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>-5.146470891238805E-09</v>
+        <v>-5.146480962667802E-09</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>4.677497130435172E-09</v>
+        <v>4.67744228031843E-09</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -14389,16 +14389,16 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>0.7848521014100441</v>
+        <v>0.7848521014100445</v>
       </c>
       <c r="O2">
-        <v>0.7848521014176205</v>
+        <v>0.7848521014176209</v>
       </c>
       <c r="P2">
-        <v>-10.40459667877252</v>
+        <v>-10.4045966787725</v>
       </c>
       <c r="Q2">
-        <v>-10.40459667698051</v>
+        <v>-10.4045966769805</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -14442,16 +14442,16 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.7848521014201459</v>
+        <v>0.7848521014201464</v>
       </c>
       <c r="O3">
-        <v>0.7848521014176205</v>
+        <v>0.7848521014176209</v>
       </c>
       <c r="P3">
-        <v>-10.40459667638317</v>
+        <v>-10.40459667638316</v>
       </c>
       <c r="Q3">
-        <v>-10.40459667698051</v>
+        <v>-10.4045966769805</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -14495,16 +14495,16 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.7848521014201459</v>
+        <v>0.7848521014201463</v>
       </c>
       <c r="O4">
-        <v>0.7848521014176205</v>
+        <v>0.7848521014176209</v>
       </c>
       <c r="P4">
         <v>-10.40459667638317</v>
       </c>
       <c r="Q4">
-        <v>-10.40459667698051</v>
+        <v>-10.4045966769805</v>
       </c>
     </row>
   </sheetData>
@@ -14584,7 +14584,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>3.617452049950389E-10</v>
+        <v>3.617436737412018E-10</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -14596,13 +14596,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>-5.146470891238805E-09</v>
+        <v>-5.146480962667802E-09</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>4.677497130435172E-09</v>
+        <v>4.67744228031843E-09</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -14614,16 +14614,16 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>0.7848521014100441</v>
+        <v>0.7848521014100445</v>
       </c>
       <c r="O2">
-        <v>0.7848521014176205</v>
+        <v>0.7848521014176209</v>
       </c>
       <c r="P2">
-        <v>-10.40459667877252</v>
+        <v>-10.4045966787725</v>
       </c>
       <c r="Q2">
-        <v>-10.40459667698051</v>
+        <v>-10.4045966769805</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -14667,16 +14667,16 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.7848521014201459</v>
+        <v>0.7848521014201464</v>
       </c>
       <c r="O3">
-        <v>0.7848521014176205</v>
+        <v>0.7848521014176209</v>
       </c>
       <c r="P3">
-        <v>-10.40459667638317</v>
+        <v>-10.40459667638316</v>
       </c>
       <c r="Q3">
-        <v>-10.40459667698051</v>
+        <v>-10.4045966769805</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -14720,16 +14720,16 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.7848521014201459</v>
+        <v>0.7848521014201463</v>
       </c>
       <c r="O4">
-        <v>0.7848521014176205</v>
+        <v>0.7848521014176209</v>
       </c>
       <c r="P4">
         <v>-10.40459667638317</v>
       </c>
       <c r="Q4">
-        <v>-10.40459667698051</v>
+        <v>-10.4045966769805</v>
       </c>
     </row>
   </sheetData>

</xml_diff>